<commit_message>
rok -> liczba użytkowników -> przychód  # do dokończenia
</commit_message>
<xml_diff>
--- a/Zeszyt1.xlsx
+++ b/Zeszyt1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27900" windowHeight="12795"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="27900" windowHeight="12795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -150,8 +150,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.31561055793095305"/>
-                  <c:y val="-5.4067297343227926E-2"/>
+                  <c:x val="-0.31561055793095316"/>
+                  <c:y val="-5.4067297343227946E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -398,23 +398,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="126778368"/>
-        <c:axId val="126792448"/>
+        <c:axId val="121797632"/>
+        <c:axId val="121811712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126778368"/>
+        <c:axId val="121797632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126792448"/>
+        <c:crossAx val="121811712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126792448"/>
+        <c:axId val="121811712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,7 +422,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126778368"/>
+        <c:crossAx val="121797632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -435,7 +435,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -561,23 +561,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="127800832"/>
-        <c:axId val="127802368"/>
+        <c:axId val="122099200"/>
+        <c:axId val="122100736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127800832"/>
+        <c:axId val="122099200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127802368"/>
+        <c:crossAx val="122100736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127802368"/>
+        <c:axId val="122100736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +585,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127800832"/>
+        <c:crossAx val="122099200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -598,7 +598,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -711,23 +711,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="127835136"/>
-        <c:axId val="127845120"/>
+        <c:axId val="122137600"/>
+        <c:axId val="122143488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127835136"/>
+        <c:axId val="122137600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127845120"/>
+        <c:crossAx val="122143488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127845120"/>
+        <c:axId val="122143488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,7 +735,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127835136"/>
+        <c:crossAx val="122137600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -748,7 +748,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -876,23 +876,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="126830080"/>
-        <c:axId val="126831616"/>
+        <c:axId val="122045952"/>
+        <c:axId val="122047488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126830080"/>
+        <c:axId val="122045952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126831616"/>
+        <c:crossAx val="122047488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126831616"/>
+        <c:axId val="122047488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +900,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126830080"/>
+        <c:crossAx val="122045952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -913,7 +913,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1043,23 +1043,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="126848000"/>
-        <c:axId val="127931136"/>
+        <c:axId val="122063872"/>
+        <c:axId val="122360576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126848000"/>
+        <c:axId val="122063872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127931136"/>
+        <c:crossAx val="122360576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127931136"/>
+        <c:axId val="122360576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1067,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126848000"/>
+        <c:crossAx val="122063872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1080,7 +1080,145 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz2!$A$1:$I$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1056</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1228</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1393</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1591</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1860</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz2!$A$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3711</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5089</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7872</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12466</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17928</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27638</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="80280960"/>
+        <c:axId val="80279424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="80280960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80279424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="80279424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80280960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1181,15 +1319,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>403412</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>26334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>165847</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1233,6 +1371,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1528,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA31" workbookViewId="0">
-      <selection activeCell="AN39" sqref="AN39"/>
+    <sheetView topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2276,13 +2449,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1">
+        <v>360</v>
+      </c>
+      <c r="B1">
+        <v>608</v>
+      </c>
+      <c r="C1">
+        <v>845</v>
+      </c>
+      <c r="D1">
+        <v>1056</v>
+      </c>
+      <c r="E1">
+        <v>1228</v>
+      </c>
+      <c r="F1">
+        <v>1393</v>
+      </c>
+      <c r="G1">
+        <v>1591</v>
+      </c>
+      <c r="H1">
+        <v>1860</v>
+      </c>
+      <c r="I1">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>777</v>
+      </c>
+      <c r="B2">
+        <v>1974</v>
+      </c>
+      <c r="C2">
+        <v>3711</v>
+      </c>
+      <c r="D2">
+        <v>5089</v>
+      </c>
+      <c r="E2">
+        <v>7872</v>
+      </c>
+      <c r="F2">
+        <v>12466</v>
+      </c>
+      <c r="G2">
+        <v>17928</v>
+      </c>
+      <c r="H2">
+        <v>27638</v>
+      </c>
+      <c r="I2">
+        <v>40653</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>